<commit_message>
updated blank space in valid case
</commit_message>
<xml_diff>
--- a/Templates/logincases_allvalid.xlsx
+++ b/Templates/logincases_allvalid.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Invalid password</t>
   </si>
   <si>
-    <t xml:space="preserve">asd</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>